<commit_message>
Versão pra teste pronta
</commit_message>
<xml_diff>
--- a/Novo(a) Planilha do Microsoft Excel.xlsx
+++ b/Novo(a) Planilha do Microsoft Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\PG\IFRAMES\Equatorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD622543-57A9-42AC-826E-2F6462C996FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7701DC3D-CCBD-48AA-82C5-8898DEE15BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="4305" windowWidth="22635" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="4620" windowWidth="22635" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>DESPESA</t>
   </si>
@@ -87,7 +87,34 @@
     <t>A1</t>
   </si>
   <si>
-    <t>HOPE</t>
+    <t>in_stock</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>DESPE_SUFR</t>
+  </si>
+  <si>
+    <t>HOPE 1</t>
+  </si>
+  <si>
+    <t>HOPE 2</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>D003</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>HOPE 3</t>
+  </si>
+  <si>
+    <t>INVEST</t>
   </si>
 </sst>
 </file>
@@ -458,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>3333</v>
+        <v>1111</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -547,10 +574,10 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>1</v>
@@ -559,6 +586,90 @@
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2222</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>333</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>